<commit_message>
Update BURN DOWN CHART SPRINT 3.xlsx
</commit_message>
<xml_diff>
--- a/complements/documentacion/BURN DOWN CHART SPRINT 3.xlsx
+++ b/complements/documentacion/BURN DOWN CHART SPRINT 3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CONSULTORIO-ODONTOLOGICO\complements\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF5B13F-4115-4845-9204-7F970F01A343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580BD10F-7A94-4337-B033-721BA2EC91A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64DE9620-C2DA-42C7-8FFF-32EF6034B830}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{64DE9620-C2DA-42C7-8FFF-32EF6034B830}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,19 +35,28 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -109,21 +118,6 @@
     <t>PRONÓSTICO</t>
   </si>
   <si>
-    <t>DEVELOPER 1</t>
-  </si>
-  <si>
-    <t>DEVELOPER 2</t>
-  </si>
-  <si>
-    <t>DEVELOPER 3</t>
-  </si>
-  <si>
-    <t>DEVELOPER 4</t>
-  </si>
-  <si>
-    <t>DEVELOPER 5</t>
-  </si>
-  <si>
     <t>ESFUERZO TOTAL</t>
   </si>
   <si>
@@ -131,6 +125,21 @@
   </si>
   <si>
     <t>ESFUERZO DISPONIBLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jose </t>
+  </si>
+  <si>
+    <t>Camila</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Caro</t>
   </si>
 </sst>
 </file>
@@ -219,10 +228,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,34 +660,34 @@
                   <c:v>175</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>175</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>175</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>175</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>175</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>175</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>175</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>175</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>175</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>175</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>175</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1844,38 +1853,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BF7B20-EDD3-46B6-BE9E-C2276AFB3164}">
   <dimension ref="B2:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1896,7 +1905,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>1</v>
       </c>
@@ -1922,7 +1931,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>2</v>
       </c>
@@ -1944,10 +1953,10 @@
       </c>
       <c r="L6" s="6">
         <f>_xlfn.NUMBERVALUE(Hoja2!J5)</f>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>3</v>
       </c>
@@ -1969,10 +1978,10 @@
       </c>
       <c r="L7" s="6">
         <f>_xlfn.NUMBERVALUE(Hoja2!J6)</f>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>4</v>
       </c>
@@ -1993,10 +2002,10 @@
       </c>
       <c r="L8" s="6">
         <f>_xlfn.NUMBERVALUE(Hoja2!J7)</f>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>5</v>
       </c>
@@ -2017,10 +2026,10 @@
       </c>
       <c r="L9" s="6">
         <f>_xlfn.NUMBERVALUE(Hoja2!J8)</f>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>6</v>
       </c>
@@ -2042,10 +2051,10 @@
       </c>
       <c r="L10" s="6">
         <f>_xlfn.NUMBERVALUE(Hoja2!J9)</f>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>7</v>
       </c>
@@ -2067,17 +2076,17 @@
       </c>
       <c r="L11" s="6">
         <f>_xlfn.NUMBERVALUE(Hoja2!J10)</f>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <v>8</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <f>HORAS_DEL_TRABAJO_POR_DIA/DIAS_DE_TRABAJADOS</f>
         <v>0.35</v>
       </c>
@@ -2092,10 +2101,10 @@
       </c>
       <c r="L12" s="6">
         <f>_xlfn.NUMBERVALUE(Hoja2!J11)</f>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>9</v>
       </c>
@@ -2117,10 +2126,10 @@
       </c>
       <c r="L13" s="6">
         <f>_xlfn.NUMBERVALUE(Hoja2!J12)</f>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <v>10</v>
       </c>
@@ -2142,10 +2151,10 @@
       </c>
       <c r="L14" s="6">
         <f>_xlfn.NUMBERVALUE(Hoja2!J13)</f>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="I15" s="3">
         <v>10</v>
       </c>
@@ -2157,10 +2166,10 @@
       </c>
       <c r="L15" s="6">
         <f>_xlfn.NUMBERVALUE(Hoja2!J13)</f>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="L16" s="2"/>
     </row>
   </sheetData>
@@ -2176,56 +2185,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96468608-FC59-4B58-88BD-6D2B1FDD919E}">
   <dimension ref="B3:J17"/>
   <sheetViews>
-    <sheetView zoomScale="65" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="2" max="7" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
       <c r="H4" s="3">
         <f>SUM(C4:G4)</f>
         <v>0</v>
@@ -2239,51 +2258,59 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3">
         <f t="shared" ref="H5:H13" si="1">SUM(C5:G5)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I5" s="3">
         <f>I4+H5</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" si="0"/>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="C6" s="3">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3">
+        <v>5</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I6" s="3">
         <f t="shared" ref="I6:I13" si="2">I5+H6</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" si="0"/>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>4</v>
       </c>
@@ -2298,14 +2325,14 @@
       </c>
       <c r="I7" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" si="0"/>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>5</v>
       </c>
@@ -2320,14 +2347,14 @@
       </c>
       <c r="I8" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" si="0"/>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>6</v>
       </c>
@@ -2342,14 +2369,14 @@
       </c>
       <c r="I9" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" si="0"/>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>7</v>
       </c>
@@ -2364,14 +2391,14 @@
       </c>
       <c r="I10" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="0"/>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>8</v>
       </c>
@@ -2386,14 +2413,14 @@
       </c>
       <c r="I11" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" si="0"/>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <v>9</v>
       </c>
@@ -2408,14 +2435,14 @@
       </c>
       <c r="I12" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" si="0"/>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>10</v>
       </c>
@@ -2432,25 +2459,25 @@
       </c>
       <c r="I13" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" si="0"/>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E14" s="7"/>
       <c r="H14" s="7">
         <f>SUM(H4:H13)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J14" s="7">
         <f>SUM(J4:J13)</f>
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17">
         <f ca="1">RANDBETWEEN(4,8)</f>
         <v>4</v>

</xml_diff>

<commit_message>
Implementación de horas en el burn down chart
Se esta implementando mis horas en el burn down chart en un momento lo voy a subir tambien de kevin
</commit_message>
<xml_diff>
--- a/complements/documentacion/BURN DOWN CHART SPRINT 3.xlsx
+++ b/complements/documentacion/BURN DOWN CHART SPRINT 3.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CONSULTORIO-ODONTOLOGICO\complements\documentacion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF5B13F-4115-4845-9204-7F970F01A343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64DE9620-C2DA-42C7-8FFF-32EF6034B830}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +24,7 @@
     <definedName name="TOTAL_HORAS_DISPONIBLES">Hoja1!$D$10</definedName>
     <definedName name="TOTAL_PENDIENTE">Hoja2!$I$4:$I$13</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -115,15 +109,6 @@
     <t>DEVELOPER 2</t>
   </si>
   <si>
-    <t>DEVELOPER 3</t>
-  </si>
-  <si>
-    <t>DEVELOPER 4</t>
-  </si>
-  <si>
-    <t>DEVELOPER 5</t>
-  </si>
-  <si>
     <t>ESFUERZO TOTAL</t>
   </si>
   <si>
@@ -132,11 +117,20 @@
   <si>
     <t>ESFUERZO DISPONIBLE</t>
   </si>
+  <si>
+    <t>IVAN</t>
+  </si>
+  <si>
+    <t>KEVIN</t>
+  </si>
+  <si>
+    <t>CAROLYN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -219,10 +213,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -242,9 +236,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-BO"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -287,6 +281,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -295,25 +290,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-BO"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -438,7 +414,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C7EB-4620-AB5E-456FC4C633E9}"/>
             </c:ext>
@@ -561,7 +537,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C7EB-4620-AB5E-456FC4C633E9}"/>
             </c:ext>
@@ -648,43 +624,43 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>175</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>175</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>175</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>175</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>175</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>175</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>175</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>175</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>175</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>175</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>175</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-C7EB-4620-AB5E-456FC4C633E9}"/>
             </c:ext>
@@ -698,12 +674,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="146763119"/>
-        <c:axId val="146781423"/>
+        <c:axId val="167367424"/>
+        <c:axId val="167368960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146763119"/>
+        <c:axId val="167367424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -764,7 +741,7 @@
             <a:endParaRPr lang="es-BO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146781423"/>
+        <c:crossAx val="167368960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -772,7 +749,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146781423"/>
+        <c:axId val="167368960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -833,7 +810,7 @@
             <a:endParaRPr lang="es-BO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146763119"/>
+        <c:crossAx val="167367424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -847,6 +824,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1524,7 +1502,7 @@
         <xdr:cNvPr id="4" name="Gráfico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27FCDC1B-27F6-4A78-BD70-FEDEC5E4C6E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{27FCDC1B-27F6-4A78-BD70-FEDEC5E4C6E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1834,17 +1812,17 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BF7B20-EDD3-46B6-BE9E-C2276AFB3164}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:D14"/>
     </sheetView>
   </sheetViews>
@@ -1856,24 +1834,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
@@ -1917,9 +1895,9 @@
         <f t="array" ref="K5:K15">TOTAL_HORAS_DISPONIBLES-(DIAS_DEL_SPRINT*PORCENTAJE_DIARIO_DE_HORAS_DISPONIBLES)</f>
         <v>175</v>
       </c>
-      <c r="L5" s="6">
-        <f>_xlfn.NUMBERVALUE(Hoja2!J4)</f>
-        <v>175</v>
+      <c r="L5" s="6" t="e">
+        <f ca="1">_xlfn.NUMBERVALUE(Hoja2!J4)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1942,9 +1920,9 @@
       <c r="K6" s="6">
         <v>168.875</v>
       </c>
-      <c r="L6" s="6">
-        <f>_xlfn.NUMBERVALUE(Hoja2!J5)</f>
-        <v>175</v>
+      <c r="L6" s="6" t="e">
+        <f ca="1">_xlfn.NUMBERVALUE(Hoja2!J5)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1967,9 +1945,9 @@
       <c r="K7" s="6">
         <v>162.75</v>
       </c>
-      <c r="L7" s="6">
-        <f>_xlfn.NUMBERVALUE(Hoja2!J6)</f>
-        <v>175</v>
+      <c r="L7" s="6" t="e">
+        <f ca="1">_xlfn.NUMBERVALUE(Hoja2!J6)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1991,9 +1969,9 @@
       <c r="K8" s="6">
         <v>156.625</v>
       </c>
-      <c r="L8" s="6">
-        <f>_xlfn.NUMBERVALUE(Hoja2!J7)</f>
-        <v>175</v>
+      <c r="L8" s="6" t="e">
+        <f ca="1">_xlfn.NUMBERVALUE(Hoja2!J7)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2015,9 +1993,9 @@
       <c r="K9" s="6">
         <v>150.5</v>
       </c>
-      <c r="L9" s="6">
-        <f>_xlfn.NUMBERVALUE(Hoja2!J8)</f>
-        <v>175</v>
+      <c r="L9" s="6" t="e">
+        <f ca="1">_xlfn.NUMBERVALUE(Hoja2!J8)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2040,9 +2018,9 @@
       <c r="K10" s="6">
         <v>144.375</v>
       </c>
-      <c r="L10" s="6">
-        <f>_xlfn.NUMBERVALUE(Hoja2!J9)</f>
-        <v>175</v>
+      <c r="L10" s="6" t="e">
+        <f ca="1">_xlfn.NUMBERVALUE(Hoja2!J9)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2065,9 +2043,9 @@
       <c r="K11" s="6">
         <v>138.25</v>
       </c>
-      <c r="L11" s="6">
-        <f>_xlfn.NUMBERVALUE(Hoja2!J10)</f>
-        <v>175</v>
+      <c r="L11" s="6" t="e">
+        <f ca="1">_xlfn.NUMBERVALUE(Hoja2!J10)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2077,7 +2055,7 @@
       <c r="C12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <f>HORAS_DEL_TRABAJO_POR_DIA/DIAS_DE_TRABAJADOS</f>
         <v>0.35</v>
       </c>
@@ -2090,9 +2068,9 @@
       <c r="K12" s="6">
         <v>132.125</v>
       </c>
-      <c r="L12" s="6">
-        <f>_xlfn.NUMBERVALUE(Hoja2!J11)</f>
-        <v>175</v>
+      <c r="L12" s="6" t="e">
+        <f ca="1">_xlfn.NUMBERVALUE(Hoja2!J11)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2115,9 +2093,9 @@
       <c r="K13" s="6">
         <v>126</v>
       </c>
-      <c r="L13" s="6">
-        <f>_xlfn.NUMBERVALUE(Hoja2!J12)</f>
-        <v>175</v>
+      <c r="L13" s="6" t="e">
+        <f ca="1">_xlfn.NUMBERVALUE(Hoja2!J12)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2140,9 +2118,9 @@
       <c r="K14" s="6">
         <v>119.875</v>
       </c>
-      <c r="L14" s="6">
-        <f>_xlfn.NUMBERVALUE(Hoja2!J13)</f>
-        <v>175</v>
+      <c r="L14" s="6" t="e">
+        <f ca="1">_xlfn.NUMBERVALUE(Hoja2!J13)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
@@ -2155,9 +2133,9 @@
       <c r="K15" s="6">
         <v>113.75</v>
       </c>
-      <c r="L15" s="6">
-        <f>_xlfn.NUMBERVALUE(Hoja2!J13)</f>
-        <v>175</v>
+      <c r="L15" s="6" t="e">
+        <f ca="1">_xlfn.NUMBERVALUE(Hoja2!J13)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
@@ -2173,11 +2151,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96468608-FC59-4B58-88BD-6D2B1FDD919E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J17"/>
   <sheetViews>
-    <sheetView zoomScale="65" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2185,7 +2163,7 @@
     <col min="2" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
@@ -2199,22 +2177,22 @@
         <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
@@ -2224,8 +2202,12 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
       <c r="H4" s="3">
         <f>SUM(C4:G4)</f>
         <v>0</v>
@@ -2246,8 +2228,12 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
       <c r="H5" s="3">
         <f t="shared" ref="H5:H13" si="1">SUM(C5:G5)</f>
         <v>0</v>
@@ -2269,18 +2255,20 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3">
+        <v>2</v>
+      </c>
       <c r="H6" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I6" s="3">
         <f t="shared" ref="I6:I13" si="2">I5+H6</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" si="0"/>
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -2291,18 +2279,20 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="G7" s="3">
+        <v>8</v>
+      </c>
       <c r="H7" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" si="0"/>
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -2313,18 +2303,20 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3">
+        <v>7.5</v>
+      </c>
       <c r="H8" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="I8" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" si="0"/>
-        <v>175</v>
+        <v>157.5</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -2335,18 +2327,20 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="G9" s="3">
+        <v>2</v>
+      </c>
       <c r="H9" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I9" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>19.5</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" si="0"/>
-        <v>175</v>
+        <v>155.5</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -2357,18 +2351,20 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="3">
+        <v>8.5</v>
+      </c>
       <c r="H10" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="0"/>
-        <v>175</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -2379,18 +2375,20 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="3">
+        <v>9.5</v>
+      </c>
       <c r="H11" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="I11" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>37.5</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" si="0"/>
-        <v>175</v>
+        <v>137.5</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -2401,18 +2399,20 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3">
+        <v>3.5</v>
+      </c>
       <c r="H12" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="I12" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" si="0"/>
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -2432,28 +2432,28 @@
       </c>
       <c r="I13" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" si="0"/>
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E14" s="7"/>
       <c r="H14" s="7">
         <f>SUM(H4:H13)</f>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="J14" s="7">
         <f>SUM(J4:J13)</f>
-        <v>1750</v>
+        <v>1553.5</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17">
         <f ca="1">RANDBETWEEN(4,8)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IMPLEMENTACION DEL TERCER SPRINT
CAMBIOS REALIZADOS
</commit_message>
<xml_diff>
--- a/complements/documentacion/BURN DOWN CHART SPRINT 3.xlsx
+++ b/complements/documentacion/BURN DOWN CHART SPRINT 3.xlsx
@@ -8,26 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CONSULTORIO-ODONTOLOGICO\complements\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06058D6-A18D-4A80-AA9B-407EE84432D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8E6C9C-F14E-4826-B4F8-D17890DA2D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64DE9620-C2DA-42C7-8FFF-32EF6034B830}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{64DE9620-C2DA-42C7-8FFF-32EF6034B830}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DIAS_DE_TRABAJADOS">Hoja1!$D$7</definedName>
-    <definedName name="DIAS_DEL_SPRINT">Hoja1!$I$5:$I$15</definedName>
-    <definedName name="FECHA_DE_FINAL_DEL_SPRINT">Hoja1!$D$6</definedName>
-    <definedName name="FECHA_DE_INICIO_DEL_SPRINT">Hoja1!$D$5</definedName>
-    <definedName name="HORAS_DEL_TRABAJO_POR_DIA">Hoja1!$D$9</definedName>
-    <definedName name="HORAS_PRODUCTIVAS">Hoja1!$D$13</definedName>
-    <definedName name="PORCENTAJE_DE_HORAS_DISPONIBLES">Hoja1!$D$11</definedName>
-    <definedName name="PORCENTAJE_DE_PRODUCTIVIDA">Hoja1!$D$12</definedName>
-    <definedName name="PORCENTAJE_DIARIO_DE_HORAS_DISPONIBLES">Hoja1!$D$14</definedName>
-    <definedName name="TAMAÑO_DEL_EQUIPO">Hoja1!$D$8</definedName>
-    <definedName name="TOTAL_HORAS_DISPONIBLES">Hoja1!$D$10</definedName>
+    <definedName name="DIAS_DE_TRABAJADOS">Hoja1!$D$8</definedName>
+    <definedName name="DIAS_DEL_SPRINT">Hoja1!$I$6:$I$16</definedName>
+    <definedName name="FECHA_DE_FINAL_DEL_SPRINT">Hoja1!$D$7</definedName>
+    <definedName name="FECHA_DE_INICIO_DEL_SPRINT">Hoja1!$D$6</definedName>
+    <definedName name="HORAS_DEL_TRABAJO_POR_DIA">Hoja1!$D$10</definedName>
+    <definedName name="HORAS_PRODUCTIVAS">Hoja1!$D$14</definedName>
+    <definedName name="PORCENTAJE_DE_HORAS_DISPONIBLES">Hoja1!$D$12</definedName>
+    <definedName name="PORCENTAJE_DE_PRODUCTIVIDA">Hoja1!$D$13</definedName>
+    <definedName name="PORCENTAJE_DIARIO_DE_HORAS_DISPONIBLES">Hoja1!$D$15</definedName>
+    <definedName name="TAMAÑO_DEL_EQUIPO">Hoja1!$D$9</definedName>
+    <definedName name="TOTAL_HORAS_DISPONIBLES">Hoja1!$D$11</definedName>
     <definedName name="TOTAL_PENDIENTE">Hoja2!$I$4:$I$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -35,19 +35,28 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -62,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>GRÁFICA DE TRABAJO PENDIENTE (BURN DOWN CHART)</t>
   </si>
@@ -132,12 +141,21 @@
   <si>
     <t>CAROLYN</t>
   </si>
+  <si>
+    <t>GRÁFICA DE TRABAJO PENDIENTE</t>
+  </si>
+  <si>
+    <t>COORDINACION DE TRABAJO</t>
+  </si>
+  <si>
+    <t>TABLA DE PROGRESO DE TRABAJO POR INTEGRANTES</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,16 +176,54 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -191,14 +247,40 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -206,22 +288,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -326,7 +440,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$J$4</c:f>
+              <c:f>Hoja1!$J$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -355,7 +469,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$I$5:$I$15</c:f>
+              <c:f>Hoja1!$I$6:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -397,7 +511,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$J$5:$J$15</c:f>
+              <c:f>Hoja1!$J$6:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -449,7 +563,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$K$4</c:f>
+              <c:f>Hoja1!$K$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -478,7 +592,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$I$5:$I$15</c:f>
+              <c:f>Hoja1!$I$6:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -520,7 +634,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$K$5:$K$15</c:f>
+              <c:f>Hoja1!$K$6:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -572,7 +686,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$L$4</c:f>
+              <c:f>Hoja1!$L$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -601,7 +715,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$I$5:$I$15</c:f>
+              <c:f>Hoja1!$I$6:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -643,7 +757,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$L$5:$L$15</c:f>
+              <c:f>Hoja1!$L$6:$L$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -663,22 +777,22 @@
                   <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>155</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>155</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>155</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>155</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>155</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>155</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1510,13 +1624,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1223433</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1842,10 +1956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BF7B20-EDD3-46B6-BE9E-C2276AFB3164}">
-  <dimension ref="B2:L16"/>
+  <dimension ref="B2:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1853,630 +1967,702 @@
     <col min="2" max="2" width="4.28515625" customWidth="1"/>
     <col min="3" max="3" width="27.140625" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="3" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L5" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
+    <row r="6" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D6" s="7">
         <v>45243</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I6" s="12">
         <v>0</v>
       </c>
-      <c r="J5" s="6" cm="1">
-        <f t="array" ref="J5:J15">HORAS_PRODUCTIVAS-(DIAS_DEL_SPRINT*PORCENTAJE_DIARIO_DE_HORAS_DISPONIBLES)</f>
+      <c r="J6" s="13" cm="1">
+        <f t="array" ref="J6:J16">HORAS_PRODUCTIVAS-(DIAS_DEL_SPRINT*PORCENTAJE_DIARIO_DE_HORAS_DISPONIBLES)</f>
         <v>61.249999999999993</v>
       </c>
-      <c r="K5" s="6" cm="1">
-        <f t="array" ref="K5:K15">TOTAL_HORAS_DISPONIBLES-(DIAS_DEL_SPRINT*PORCENTAJE_DIARIO_DE_HORAS_DISPONIBLES)</f>
+      <c r="K6" s="13" cm="1">
+        <f t="array" ref="K6:K16">TOTAL_HORAS_DISPONIBLES-(DIAS_DEL_SPRINT*PORCENTAJE_DIARIO_DE_HORAS_DISPONIBLES)</f>
         <v>175</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L6" s="13">
         <f>_xlfn.NUMBERVALUE(Hoja2!J4)</f>
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
+    <row r="7" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="5">
-        <f>WORKDAY(D5,9)</f>
+      <c r="D7" s="7">
+        <f>WORKDAY(D6,9)</f>
         <v>45254</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I7" s="12">
         <v>1</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J7" s="13">
         <v>55.124999999999993</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K7" s="13">
         <v>168.875</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L7" s="13">
         <f>_xlfn.NUMBERVALUE(Hoja2!J5)</f>
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
+    <row r="8" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="5">
         <v>3</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="3">
-        <f>NETWORKDAYS(D5,D6)</f>
+      <c r="D8" s="8">
+        <f>NETWORKDAYS(D6,D7)</f>
         <v>10</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I8" s="12">
         <v>2</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J8" s="13">
         <v>48.999999999999993</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K8" s="13">
         <v>162.75</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L8" s="13">
         <f>_xlfn.NUMBERVALUE(Hoja2!J6)</f>
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
+    <row r="9" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="5">
         <v>4</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D9" s="8">
         <v>5</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I9" s="12">
         <v>3</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J9" s="13">
         <v>42.875</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K9" s="13">
         <v>156.625</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L9" s="13">
         <f>_xlfn.NUMBERVALUE(Hoja2!J7)</f>
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3">
+    <row r="10" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="5">
         <v>5</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D10" s="8">
         <v>3.5</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I10" s="12">
         <v>4</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J10" s="13">
         <v>36.75</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K10" s="13">
         <v>150.5</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L10" s="13">
         <f>_xlfn.NUMBERVALUE(Hoja2!J8)</f>
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3">
+    <row r="11" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
         <v>6</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D11" s="8">
         <f>DIAS_DE_TRABAJADOS*TAMAÑO_DEL_EQUIPO*HORAS_DEL_TRABAJO_POR_DIA</f>
         <v>175</v>
       </c>
-      <c r="I10" s="3">
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="I11" s="12">
         <v>5</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J11" s="13">
         <v>30.624999999999996</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K11" s="13">
         <v>144.375</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L11" s="13">
         <f>_xlfn.NUMBERVALUE(Hoja2!J9)</f>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="5">
         <v>7</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D12" s="8">
         <f>TOTAL_HORAS_DISPONIBLES/HORAS_DEL_TRABAJO_POR_DIA</f>
         <v>50</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I12" s="12">
         <v>6</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J12" s="13">
         <v>24.5</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K12" s="13">
         <v>138.25</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L12" s="13">
         <f>_xlfn.NUMBERVALUE(Hoja2!J10)</f>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
         <v>8</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D13" s="9">
         <f>HORAS_DEL_TRABAJO_POR_DIA/DIAS_DE_TRABAJADOS</f>
         <v>0.35</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I13" s="12">
         <v>7</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J13" s="13">
         <v>18.375</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K13" s="13">
         <v>132.125</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L13" s="13">
         <f>_xlfn.NUMBERVALUE(Hoja2!J11)</f>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="5">
         <v>9</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D14" s="8">
         <f>TOTAL_HORAS_DISPONIBLES*PORCENTAJE_DE_PRODUCTIVIDA</f>
         <v>61.249999999999993</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I14" s="12">
         <v>8</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J14" s="13">
         <v>12.25</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K14" s="13">
         <v>126</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L14" s="13">
         <f>_xlfn.NUMBERVALUE(Hoja2!J12)</f>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
         <v>10</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D15" s="8">
         <f>HORAS_PRODUCTIVAS/DIAS_DE_TRABAJADOS</f>
         <v>6.1249999999999991</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I15" s="12">
         <v>9</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J15" s="13">
         <v>6.125</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K15" s="13">
         <v>119.875</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L15" s="13">
         <f>_xlfn.NUMBERVALUE(Hoja2!J13)</f>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="I15" s="3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I16" s="12">
         <v>10</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J16" s="13">
         <v>0</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K16" s="13">
         <v>113.75</v>
       </c>
-      <c r="L15" s="6">
+      <c r="L16" s="13">
         <f>_xlfn.NUMBERVALUE(Hoja2!J13)</f>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L16" s="2"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L17" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:H3"/>
+  <mergeCells count="3">
+    <mergeCell ref="B2:H4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="I4:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96468608-FC59-4B58-88BD-6D2B1FDD919E}">
-  <dimension ref="B3:J17"/>
+  <dimension ref="B2:K18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="7" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="16"/>
+    </row>
+    <row r="3" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
+      <c r="B4" s="18">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="18">
         <v>0</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="18">
         <v>0</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3">
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18">
         <f>SUM(C4:G4)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="18">
         <f>H4</f>
         <v>0</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="18">
         <f t="shared" ref="J4:J13" si="0">TOTAL_HORAS_DISPONIBLES-I4</f>
         <v>175</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
+      <c r="B5" s="18">
         <v>2</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="18">
         <v>1</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="18">
         <v>1</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3">
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18">
         <f t="shared" ref="H5:H13" si="1">SUM(C5:G5)</f>
         <v>2</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="18">
         <f>I4+H5</f>
         <v>2</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="18">
         <f t="shared" si="0"/>
         <v>173</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
+      <c r="B6" s="18">
         <v>3</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="18">
         <v>5</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="18">
         <v>5</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3">
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="18">
         <f t="shared" ref="I6:I13" si="2">I5+H6</f>
         <v>12</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="18">
         <f t="shared" si="0"/>
         <v>163</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
+      <c r="B7" s="18">
         <v>4</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="18">
         <v>1</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="18">
         <v>1</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3">
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="18">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="18">
         <f t="shared" si="0"/>
         <v>161</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
+      <c r="B8" s="18">
         <v>5</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="18">
         <v>3</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="18">
         <v>3</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3">
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="18">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="18">
         <f t="shared" si="0"/>
         <v>155</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="3">
+      <c r="B9" s="18">
         <v>6</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3">
+      <c r="C9" s="18">
+        <v>6</v>
+      </c>
+      <c r="D9" s="18">
+        <v>2</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I9" s="18">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="J9" s="18">
+        <f t="shared" si="0"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="18">
+        <v>7</v>
+      </c>
+      <c r="C10" s="18">
+        <v>6</v>
+      </c>
+      <c r="D10" s="18">
+        <v>2</v>
+      </c>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I10" s="18">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="J10" s="18">
+        <f t="shared" si="0"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="18">
+        <v>8</v>
+      </c>
+      <c r="C11" s="18">
+        <v>4</v>
+      </c>
+      <c r="D11" s="18">
+        <v>1</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I11" s="18">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="J11" s="18">
+        <f t="shared" si="0"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="18">
+        <v>9</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I12" s="18">
         <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="J9" s="3">
+        <v>41</v>
+      </c>
+      <c r="J12" s="18">
         <f t="shared" si="0"/>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="3">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="18">
+        <v>10</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18">
+        <v>0</v>
+      </c>
+      <c r="H13" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I13" s="18">
         <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="J10" s="3">
+        <v>41</v>
+      </c>
+      <c r="J13" s="18">
         <f t="shared" si="0"/>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
-        <v>8</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="3">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="J11" s="3">
-        <f t="shared" si="0"/>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="3">
-        <v>9</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="3">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="J12" s="3">
-        <f t="shared" si="0"/>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="3">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="3">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="J13" s="3">
-        <f t="shared" si="0"/>
-        <v>155</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E14" s="7"/>
-      <c r="H14" s="7">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="18">
         <f>SUM(H4:H13)</f>
-        <v>20</v>
-      </c>
-      <c r="J14" s="7">
+        <v>41</v>
+      </c>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18">
         <f>SUM(J4:J13)</f>
-        <v>1602</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D17">
         <f ca="1">RANDBETWEEN(4,8)</f>
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:J2"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>